<commit_message>
Add warnings modal and object list.
</commit_message>
<xml_diff>
--- a/test-files/matrix-modifications/extra-data-random-cell-network-only-output.xlsx
+++ b/test-files/matrix-modifications/extra-data-random-cell-network-only-output.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="759" firstSheet="6" activeTab="8"/>
@@ -5934,7 +5934,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7432,6 +7432,11 @@
         <v>0</v>
       </c>
       <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="L29">
         <v>0</v>
       </c>
     </row>

</xml_diff>